<commit_message>
reverted migrations new DB model
</commit_message>
<xml_diff>
--- a/database/DBmodel.xlsx
+++ b/database/DBmodel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\LaravelMediaDB\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E594AE9A-A549-4AFE-8E43-8A2429E41143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2687212D-8444-49FC-B084-14565626A66D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14985" yWindow="3855" windowWidth="20805" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5055" yWindow="2910" windowWidth="20805" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated excel added redirect
</commit_message>
<xml_diff>
--- a/database/DBmodel.xlsx
+++ b/database/DBmodel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\LaravelMediaDB\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94962135-1AB5-4AE5-A3F7-94C02887C45F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A4C4D8-E2F6-4B8A-BFC7-CABB3831506E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5055" yWindow="2910" windowWidth="20805" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23010" yWindow="855" windowWidth="20805" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>users</t>
   </si>
@@ -81,9 +81,6 @@
     <t>collection_id</t>
   </si>
   <si>
-    <t>seasons</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -91,6 +88,15 @@
   </si>
   <si>
     <t>episodes</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>subtype</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -474,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -487,21 +493,18 @@
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -511,36 +514,46 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new migrations with tags
</commit_message>
<xml_diff>
--- a/database/DBmodel.xlsx
+++ b/database/DBmodel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\LaravelMediaDB\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b615630e0e5e78f2/3.Repositories/2020/LaravelMediaDB/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9796106F-C58B-4AA0-A8FC-AAA4B1978BF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9796106F-C58B-4AA0-A8FC-AAA4B1978BF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0673374B-7B5E-4B47-BCE4-8175C024C52A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>users</t>
   </si>
@@ -78,9 +78,6 @@
     <t>index</t>
   </si>
   <si>
-    <t>author</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
   </si>
   <si>
     <t>author_id</t>
-  </si>
-  <si>
-    <t>tag</t>
   </si>
   <si>
     <t>size</t>
@@ -162,7 +156,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -443,10 +437,10 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
@@ -470,16 +464,16 @@
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -493,16 +487,16 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -510,16 +504,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
@@ -533,7 +527,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -549,7 +543,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -584,7 +578,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>